<commit_message>
New screenshots for design chapter
</commit_message>
<xml_diff>
--- a/Evaluation/Evaluation.xlsx
+++ b/Evaluation/Evaluation.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="13380" yWindow="0" windowWidth="15420" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="Sentence Stats" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Matrix!$A$1:$U$20</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="25">
   <si>
     <t>The Guardian</t>
   </si>
@@ -96,6 +97,15 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Not in</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>Not In</t>
   </si>
 </sst>
 </file>
@@ -192,7 +202,97 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -260,6 +360,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1327,6 +1437,1100 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sentence Stats'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Not in</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sentence Stats'!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>BBC News</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BBC Sport</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bloomberg</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Business Insider UK</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CNBC</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CNN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Cricinfo</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ESPN</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FourFourTwo</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Metro</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Newsweek</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Reuters</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>The Daily Mail</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>The Guardian</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>The Independent</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>The Mirror</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Telegraph</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Washington Post</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Times of India</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sentence Stats'!$B$3:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>22.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.58</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.82</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.39</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26.07</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22.31</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.35</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26.63</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.88</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>29.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22.42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sentence Stats'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>In</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sentence Stats'!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>BBC News</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BBC Sport</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bloomberg</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Business Insider UK</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CNBC</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CNN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Cricinfo</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ESPN</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FourFourTwo</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Metro</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Newsweek</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Reuters</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>The Daily Mail</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>The Guardian</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>The Independent</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>The Mirror</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Telegraph</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Washington Post</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Times of India</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sentence Stats'!$C$3:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>20.14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.42</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.06</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.92</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.88</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23.94</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26.45</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.33</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.01</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24.13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.06</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.04</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27.26</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="43130512"/>
+        <c:axId val="43180160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="43130512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="43180160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="43180160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="43130512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sentence Stats'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Not in</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sentence Stats'!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>BBC News</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BBC Sport</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bloomberg</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Business Insider UK</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CNBC</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CNN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Cricinfo</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ESPN</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FourFourTwo</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Metro</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Newsweek</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Reuters</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>The Daily Mail</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>The Guardian</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>The Independent</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>The Mirror</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Telegraph</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Washington Post</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Times of India</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sentence Stats'!$B$3:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>22.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.58</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.82</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.39</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26.07</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22.31</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.35</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26.63</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.88</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>29.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22.42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sentence Stats'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>In</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sentence Stats'!$A$3:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>BBC News</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BBC Sport</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bloomberg</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Business Insider UK</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CNBC</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CNN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Cricinfo</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ESPN</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FourFourTwo</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Metro</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Newsweek</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Reuters</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>The Daily Mail</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>The Guardian</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>The Independent</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>The Mirror</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>The Telegraph</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>The Washington Post</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Times of India</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sentence Stats'!$C$3:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>20.14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.42</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.06</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.92</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.88</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23.94</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26.45</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.33</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.01</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24.13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.06</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.04</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27.26</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="7429648"/>
+        <c:axId val="46586352"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="7429648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="46586352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="46586352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="7429648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1447,6 +2651,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
   <cs:axisTitle>
@@ -2892,6 +4176,1027 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3011,6 +5316,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>615950</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3284,8 +5654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM20"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="AP1" zoomScale="53" zoomScaleNormal="53" zoomScalePageLayoutView="53" workbookViewId="0">
-      <selection activeCell="AU3" sqref="AU3"/>
+    <sheetView showRuler="0" topLeftCell="AP1" zoomScale="53" zoomScaleNormal="53" zoomScalePageLayoutView="53" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3611,8 +5981,8 @@
         <v>1</v>
       </c>
       <c r="AQ2" s="6">
-        <f>AVERAGE(X2:AP2)</f>
-        <v>7.2</v>
+        <f>SUM(X2:AP2)</f>
+        <v>108</v>
       </c>
       <c r="AS2" s="2" t="s">
         <v>3</v>
@@ -3690,8 +6060,8 @@
         <v>56</v>
       </c>
       <c r="BM2" s="6">
-        <f>AVERAGE(AT2:BL2)</f>
-        <v>265.95933333333335</v>
+        <f>SUM(AT2:BL2)/AQ2</f>
+        <v>36.938796296296296</v>
       </c>
     </row>
     <row r="3" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -3820,8 +6190,8 @@
         <v>21</v>
       </c>
       <c r="AQ3" s="6">
-        <f t="shared" ref="AQ3:AQ20" si="12">AVERAGE(X3:AP3)</f>
-        <v>4.4545454545454541</v>
+        <f t="shared" ref="AQ3:AQ20" si="12">SUM(X3:AP3)</f>
+        <v>49</v>
       </c>
       <c r="AS3" s="2" t="s">
         <v>8</v>
@@ -3830,9 +6200,8 @@
         <f t="shared" ref="AT3:BB20" si="13">B3*X3</f>
         <v>117.4</v>
       </c>
-      <c r="AU3" s="7" t="e">
-        <f t="shared" ref="AU3" si="14">C3*Y3</f>
-        <v>#VALUE!</v>
+      <c r="AU3" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AV3" s="7">
         <f t="shared" si="0"/>
@@ -3842,21 +6211,18 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="AX3" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY3" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AX3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AY3" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AZ3" s="7">
         <f t="shared" si="0"/>
         <v>187.5</v>
       </c>
-      <c r="BA3" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="BA3" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BB3" s="7">
         <f t="shared" si="0"/>
@@ -3870,9 +6236,8 @@
         <f t="shared" si="2"/>
         <v>33.299999999999997</v>
       </c>
-      <c r="BE3" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+      <c r="BE3" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BF3" s="7">
         <f t="shared" si="4"/>
@@ -3882,9 +6247,8 @@
         <f t="shared" si="5"/>
         <v>108.60000000000001</v>
       </c>
-      <c r="BH3" s="7" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="BH3" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BI3" s="7">
         <f t="shared" si="7"/>
@@ -3894,17 +6258,15 @@
         <f t="shared" si="8"/>
         <v>14.3</v>
       </c>
-      <c r="BK3" s="7" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BL3" s="7" t="e">
-        <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BM3" s="6" t="e">
-        <f t="shared" ref="BM3:BM20" si="15">AVERAGE(AT3:BL3)</f>
-        <v>#VALUE!</v>
+      <c r="BK3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BL3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BM3" s="6">
+        <f t="shared" ref="BM3:BM20" si="14">SUM(AT3:BL3)/AQ3</f>
+        <v>60.475510204081637</v>
       </c>
     </row>
     <row r="4" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -4034,7 +6396,7 @@
       </c>
       <c r="AQ4" s="6">
         <f t="shared" si="12"/>
-        <v>4.7857142857142856</v>
+        <v>67</v>
       </c>
       <c r="AS4" s="2" t="s">
         <v>7</v>
@@ -4047,9 +6409,8 @@
         <f t="shared" si="13"/>
         <v>118.19999999999999</v>
       </c>
-      <c r="AV4" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AV4" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AW4" s="7">
         <f t="shared" si="0"/>
@@ -4063,17 +6424,14 @@
         <f t="shared" si="0"/>
         <v>561</v>
       </c>
-      <c r="AZ4" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA4" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BB4" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AZ4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BA4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB4" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BC4" s="7">
         <f t="shared" si="1"/>
@@ -4099,9 +6457,8 @@
         <f t="shared" si="6"/>
         <v>319.79999999999995</v>
       </c>
-      <c r="BI4" s="7" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+      <c r="BI4" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BJ4" s="7">
         <f t="shared" si="8"/>
@@ -4115,9 +6472,9 @@
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="BM4" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BM4" s="6">
+        <f t="shared" si="14"/>
+        <v>55.408955223880604</v>
       </c>
     </row>
     <row r="5" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -4247,7 +6604,7 @@
       </c>
       <c r="AQ5" s="6">
         <f t="shared" si="12"/>
-        <v>6.875</v>
+        <v>110</v>
       </c>
       <c r="AS5" s="2" t="s">
         <v>9</v>
@@ -4264,9 +6621,8 @@
         <f t="shared" si="0"/>
         <v>176.10000000000002</v>
       </c>
-      <c r="AW5" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AW5" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AX5" s="7">
         <f t="shared" si="0"/>
@@ -4276,17 +6632,15 @@
         <f t="shared" si="0"/>
         <v>522</v>
       </c>
-      <c r="AZ5" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AZ5" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BA5" s="7">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="BB5" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="BB5" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BC5" s="7">
         <f t="shared" si="1"/>
@@ -4328,9 +6682,9 @@
         <f t="shared" si="10"/>
         <v>71.430000000000007</v>
       </c>
-      <c r="BM5" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BM5" s="6">
+        <f t="shared" si="14"/>
+        <v>47.849636363636364</v>
       </c>
     </row>
     <row r="6" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -4460,7 +6814,7 @@
       </c>
       <c r="AQ6" s="6">
         <f t="shared" si="12"/>
-        <v>12.923076923076923</v>
+        <v>168</v>
       </c>
       <c r="AS6" s="2" t="s">
         <v>10</v>
@@ -4469,9 +6823,8 @@
         <f t="shared" si="13"/>
         <v>185.7</v>
       </c>
-      <c r="AU6" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+      <c r="AU6" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AV6" s="7">
         <f t="shared" si="0"/>
@@ -4481,25 +6834,21 @@
         <f t="shared" si="0"/>
         <v>167.67</v>
       </c>
-      <c r="AX6" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AX6" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AY6" s="7">
         <f t="shared" si="0"/>
         <v>454.6</v>
       </c>
-      <c r="AZ6" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA6" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BB6" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AZ6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BA6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB6" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BC6" s="7">
         <f t="shared" si="1"/>
@@ -4537,13 +6886,12 @@
         <f t="shared" si="9"/>
         <v>402.2</v>
       </c>
-      <c r="BL6" s="7" t="e">
-        <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BM6" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BL6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BM6" s="6">
+        <f t="shared" si="14"/>
+        <v>43.480297619047619</v>
       </c>
     </row>
     <row r="7" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -4673,7 +7021,7 @@
       </c>
       <c r="AQ7" s="6">
         <f t="shared" si="12"/>
-        <v>11.857142857142858</v>
+        <v>166</v>
       </c>
       <c r="AS7" s="2" t="s">
         <v>11</v>
@@ -4682,9 +7030,8 @@
         <f t="shared" si="13"/>
         <v>887.7</v>
       </c>
-      <c r="AU7" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+      <c r="AU7" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AV7" s="7">
         <f t="shared" si="0"/>
@@ -4698,21 +7045,17 @@
         <f t="shared" si="0"/>
         <v>545.4</v>
       </c>
-      <c r="AY7" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ7" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA7" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BB7" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AY7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AZ7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BA7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB7" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BC7" s="7">
         <f t="shared" si="1"/>
@@ -4754,9 +7097,9 @@
         <f t="shared" si="10"/>
         <v>84.63</v>
       </c>
-      <c r="BM7" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BM7" s="6">
+        <f t="shared" si="14"/>
+        <v>60.91993975903614</v>
       </c>
     </row>
     <row r="8" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -4886,58 +7229,48 @@
       </c>
       <c r="AQ8" s="6">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="AS8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AT8" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+      <c r="AT8" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AU8" s="7">
         <f t="shared" si="13"/>
         <v>112.5</v>
       </c>
-      <c r="AV8" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AW8" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AX8" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY8" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ8" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA8" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BB8" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AV8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AW8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AX8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AY8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AZ8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BA8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB8" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BC8" s="7">
         <f t="shared" si="1"/>
         <v>411.3</v>
       </c>
-      <c r="BD8" s="7" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BE8" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+      <c r="BD8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BE8" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BF8" s="7">
         <f t="shared" si="4"/>
@@ -4947,29 +7280,25 @@
         <f t="shared" si="5"/>
         <v>107.69999999999999</v>
       </c>
-      <c r="BH8" s="7" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="BH8" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BI8" s="7">
         <f t="shared" si="7"/>
         <v>116.67</v>
       </c>
-      <c r="BJ8" s="7" t="e">
-        <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BK8" s="7" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BL8" s="7" t="e">
-        <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BM8" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BJ8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BK8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BL8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BM8" s="6">
+        <f t="shared" si="14"/>
+        <v>46.972499999999997</v>
       </c>
     </row>
     <row r="9" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -5099,46 +7428,38 @@
       </c>
       <c r="AQ9" s="6">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="AS9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AT9" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AU9" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AV9" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AT9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AV9" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AW9" s="7">
         <f t="shared" si="0"/>
         <v>115.9</v>
       </c>
-      <c r="AX9" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY9" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ9" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA9" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BB9" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AX9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AY9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AZ9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BA9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB9" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BC9" s="7">
         <f t="shared" si="1"/>
@@ -5148,9 +7469,8 @@
         <f t="shared" si="2"/>
         <v>104.76</v>
       </c>
-      <c r="BE9" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+      <c r="BE9" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BF9" s="7">
         <f t="shared" si="4"/>
@@ -5160,29 +7480,24 @@
         <f t="shared" si="5"/>
         <v>87.99</v>
       </c>
-      <c r="BH9" s="7" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BI9" s="7" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BJ9" s="7" t="e">
-        <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BK9" s="7" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BL9" s="7" t="e">
-        <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BM9" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BH9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BI9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BJ9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BK9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BL9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BM9" s="6">
+        <f t="shared" si="14"/>
+        <v>49.428000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -5312,46 +7627,38 @@
       </c>
       <c r="AQ10" s="6">
         <f t="shared" si="12"/>
-        <v>5.7142857142857144</v>
+        <v>40</v>
       </c>
       <c r="AS10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AT10" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+      <c r="AT10" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AU10" s="7">
         <f t="shared" si="13"/>
         <v>142.88</v>
       </c>
-      <c r="AV10" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AW10" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AX10" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY10" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ10" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA10" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BB10" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AV10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AW10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AX10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AY10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AZ10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BA10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB10" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BC10" s="7">
         <f t="shared" si="1"/>
@@ -5361,9 +7668,8 @@
         <f t="shared" si="2"/>
         <v>131.44</v>
       </c>
-      <c r="BE10" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+      <c r="BE10" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BF10" s="7">
         <f t="shared" si="4"/>
@@ -5373,9 +7679,8 @@
         <f t="shared" si="5"/>
         <v>260.39999999999998</v>
       </c>
-      <c r="BH10" s="7" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="BH10" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BI10" s="7">
         <f t="shared" si="7"/>
@@ -5385,17 +7690,15 @@
         <f t="shared" si="8"/>
         <v>45.45</v>
       </c>
-      <c r="BK10" s="7" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BL10" s="7" t="e">
-        <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BM10" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BK10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BL10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BM10" s="6">
+        <f t="shared" si="14"/>
+        <v>47.167999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -5525,7 +7828,7 @@
       </c>
       <c r="AQ11" s="6">
         <f t="shared" si="12"/>
-        <v>10.6875</v>
+        <v>171</v>
       </c>
       <c r="AS11" s="2" t="s">
         <v>15</v>
@@ -5566,9 +7869,8 @@
         <f t="shared" si="0"/>
         <v>227.29</v>
       </c>
-      <c r="BC11" s="7" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="BC11" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BD11" s="7">
         <f t="shared" si="2"/>
@@ -5598,17 +7900,15 @@
         <f t="shared" si="8"/>
         <v>1083.42</v>
       </c>
-      <c r="BK11" s="7" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BL11" s="7" t="e">
-        <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BM11" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BK11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BL11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BM11" s="6">
+        <f t="shared" si="14"/>
+        <v>48.224502923976608</v>
       </c>
     </row>
     <row r="12" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -5738,7 +8038,7 @@
       </c>
       <c r="AQ12" s="6">
         <f t="shared" si="12"/>
-        <v>7.882352941176471</v>
+        <v>134</v>
       </c>
       <c r="AS12" s="2" t="s">
         <v>16</v>
@@ -5767,9 +8067,8 @@
         <f t="shared" si="0"/>
         <v>425.85</v>
       </c>
-      <c r="AZ12" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AZ12" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BA12" s="7">
         <f t="shared" si="0"/>
@@ -5783,9 +8082,8 @@
         <f t="shared" si="1"/>
         <v>613.9</v>
       </c>
-      <c r="BD12" s="7" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="BD12" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BE12" s="7">
         <f t="shared" si="3"/>
@@ -5819,9 +8117,9 @@
         <f t="shared" si="10"/>
         <v>50.849999999999994</v>
       </c>
-      <c r="BM12" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BM12" s="6">
+        <f t="shared" si="14"/>
+        <v>49.191417910447761</v>
       </c>
     </row>
     <row r="13" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -5951,7 +8249,7 @@
       </c>
       <c r="AQ13" s="6">
         <f t="shared" si="12"/>
-        <v>11.5</v>
+        <v>161</v>
       </c>
       <c r="AS13" s="2" t="s">
         <v>17</v>
@@ -5960,9 +8258,8 @@
         <f t="shared" si="13"/>
         <v>557.6</v>
       </c>
-      <c r="AU13" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+      <c r="AU13" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AV13" s="7">
         <f t="shared" si="0"/>
@@ -5980,17 +8277,14 @@
         <f t="shared" si="0"/>
         <v>369.95</v>
       </c>
-      <c r="AZ13" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA13" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BB13" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AZ13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BA13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB13" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BC13" s="7">
         <f t="shared" si="1"/>
@@ -6000,9 +8294,8 @@
         <f t="shared" si="2"/>
         <v>265.39999999999998</v>
       </c>
-      <c r="BE13" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+      <c r="BE13" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BF13" s="7">
         <f t="shared" si="4"/>
@@ -6032,9 +8325,9 @@
         <f t="shared" si="10"/>
         <v>471.35</v>
       </c>
-      <c r="BM13" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BM13" s="6">
+        <f t="shared" si="14"/>
+        <v>35.339068322981369</v>
       </c>
     </row>
     <row r="14" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -6164,7 +8457,7 @@
       </c>
       <c r="AQ14" s="6">
         <f t="shared" si="12"/>
-        <v>13</v>
+        <v>234</v>
       </c>
       <c r="AS14" s="2" t="s">
         <v>1</v>
@@ -6217,9 +8510,8 @@
         <f t="shared" si="3"/>
         <v>3230.76</v>
       </c>
-      <c r="BF14" s="7" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
+      <c r="BF14" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BG14" s="7">
         <f t="shared" si="5"/>
@@ -6245,9 +8537,9 @@
         <f t="shared" si="10"/>
         <v>115.66</v>
       </c>
-      <c r="BM14" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BM14" s="6">
+        <f t="shared" si="14"/>
+        <v>67.077008547008546</v>
       </c>
     </row>
     <row r="15" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -6377,7 +8669,7 @@
       </c>
       <c r="AQ15" s="6">
         <f t="shared" si="12"/>
-        <v>6.5</v>
+        <v>117</v>
       </c>
       <c r="AS15" s="2" t="s">
         <v>0</v>
@@ -6434,9 +8726,8 @@
         <f t="shared" si="4"/>
         <v>432.5</v>
       </c>
-      <c r="BG15" s="7" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
+      <c r="BG15" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BH15" s="7">
         <f t="shared" si="6"/>
@@ -6458,9 +8749,9 @@
         <f t="shared" si="10"/>
         <v>95</v>
       </c>
-      <c r="BM15" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BM15" s="6">
+        <f t="shared" si="14"/>
+        <v>59.529658119658116</v>
       </c>
     </row>
     <row r="16" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -6590,7 +8881,7 @@
       </c>
       <c r="AQ16" s="6">
         <f t="shared" si="12"/>
-        <v>12.307692307692308</v>
+        <v>160</v>
       </c>
       <c r="AS16" s="2" t="s">
         <v>4</v>
@@ -6599,9 +8890,8 @@
         <f t="shared" si="13"/>
         <v>1107.9000000000001</v>
       </c>
-      <c r="AU16" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+      <c r="AU16" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AV16" s="7">
         <f t="shared" si="0"/>
@@ -6619,17 +8909,14 @@
         <f t="shared" si="0"/>
         <v>800.25</v>
       </c>
-      <c r="AZ16" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA16" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BB16" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AZ16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BA16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB16" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BC16" s="7">
         <f t="shared" si="1"/>
@@ -6651,9 +8938,8 @@
         <f t="shared" si="5"/>
         <v>421.08000000000004</v>
       </c>
-      <c r="BH16" s="7" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="BH16" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BI16" s="7">
         <f t="shared" si="7"/>
@@ -6667,13 +8953,12 @@
         <f t="shared" si="9"/>
         <v>824</v>
       </c>
-      <c r="BL16" s="7" t="e">
-        <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BM16" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BL16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BM16" s="6">
+        <f t="shared" si="14"/>
+        <v>41.016937499999997</v>
       </c>
     </row>
     <row r="17" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -6803,7 +9088,7 @@
       </c>
       <c r="AQ17" s="6">
         <f t="shared" si="12"/>
-        <v>10.533333333333333</v>
+        <v>158</v>
       </c>
       <c r="AS17" s="2" t="s">
         <v>5</v>
@@ -6816,9 +9101,8 @@
         <f t="shared" si="13"/>
         <v>99.45</v>
       </c>
-      <c r="AV17" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="AV17" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AW17" s="7">
         <f t="shared" si="0"/>
@@ -6836,9 +9120,8 @@
         <f t="shared" si="0"/>
         <v>183.32999999999998</v>
       </c>
-      <c r="BA17" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="BA17" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BB17" s="7">
         <f t="shared" si="0"/>
@@ -6868,25 +9151,23 @@
         <f t="shared" si="6"/>
         <v>578.69999999999993</v>
       </c>
-      <c r="BI17" s="7" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+      <c r="BI17" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BJ17" s="7">
         <f t="shared" si="8"/>
         <v>469.48999999999995</v>
       </c>
-      <c r="BK17" s="7" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
+      <c r="BK17" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BL17" s="7">
         <f t="shared" si="10"/>
         <v>40.630000000000003</v>
       </c>
-      <c r="BM17" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BM17" s="6">
+        <f t="shared" si="14"/>
+        <v>49.928164556962024</v>
       </c>
     </row>
     <row r="18" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -7016,7 +9297,7 @@
       </c>
       <c r="AQ18" s="6">
         <f t="shared" si="12"/>
-        <v>10.125</v>
+        <v>162</v>
       </c>
       <c r="AS18" s="2" t="s">
         <v>2</v>
@@ -7045,13 +9326,11 @@
         <f t="shared" si="13"/>
         <v>287.36</v>
       </c>
-      <c r="AZ18" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA18" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+      <c r="AZ18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BA18" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BB18" s="7">
         <f t="shared" si="13"/>
@@ -7085,9 +9364,8 @@
         <f t="shared" si="7"/>
         <v>230.51</v>
       </c>
-      <c r="BJ18" s="7" t="e">
-        <f t="shared" si="8"/>
-        <v>#VALUE!</v>
+      <c r="BJ18" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BK18" s="7">
         <f t="shared" si="9"/>
@@ -7097,9 +9375,9 @@
         <f t="shared" si="10"/>
         <v>63.16</v>
       </c>
-      <c r="BM18" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BM18" s="6">
+        <f t="shared" si="14"/>
+        <v>41.273518518518522</v>
       </c>
     </row>
     <row r="19" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -7229,7 +9507,7 @@
       </c>
       <c r="AQ19" s="6">
         <f t="shared" si="12"/>
-        <v>6.0909090909090908</v>
+        <v>67</v>
       </c>
       <c r="AS19" s="2" t="s">
         <v>19</v>
@@ -7238,9 +9516,8 @@
         <f t="shared" si="13"/>
         <v>413.91</v>
       </c>
-      <c r="AU19" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+      <c r="AU19" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AV19" s="7">
         <f t="shared" si="13"/>
@@ -7258,21 +9535,17 @@
         <f t="shared" si="13"/>
         <v>570</v>
       </c>
-      <c r="AZ19" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA19" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BB19" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BC19" s="7" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="AZ19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BA19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BC19" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BD19" s="7">
         <f t="shared" si="2"/>
@@ -7294,25 +9567,22 @@
         <f t="shared" si="6"/>
         <v>775.84</v>
       </c>
-      <c r="BI19" s="7" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+      <c r="BI19" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BJ19" s="7">
         <f t="shared" si="8"/>
         <v>136.84</v>
       </c>
-      <c r="BK19" s="7" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BL19" s="7" t="e">
-        <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BM19" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BK19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BL19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BM19" s="6">
+        <f t="shared" si="14"/>
+        <v>58.678358208955224</v>
       </c>
     </row>
     <row r="20" spans="1:65" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -7442,7 +9712,7 @@
       </c>
       <c r="AQ20" s="6">
         <f t="shared" si="12"/>
-        <v>2.7</v>
+        <v>27</v>
       </c>
       <c r="AS20" s="2" t="s">
         <v>18</v>
@@ -7451,9 +9721,8 @@
         <f t="shared" si="13"/>
         <v>44</v>
       </c>
-      <c r="AU20" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+      <c r="AU20" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AV20" s="7">
         <f t="shared" si="13"/>
@@ -7463,29 +9732,24 @@
         <f t="shared" si="13"/>
         <v>28.57</v>
       </c>
-      <c r="AX20" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+      <c r="AX20" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="AY20" s="7">
         <f t="shared" si="13"/>
         <v>215.39999999999998</v>
       </c>
-      <c r="AZ20" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA20" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BB20" s="7" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BC20" s="7" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="AZ20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BA20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BC20" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BD20" s="7">
         <f t="shared" si="2"/>
@@ -7503,9 +9767,8 @@
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="BH20" s="7" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="BH20" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="BI20" s="7">
         <f t="shared" si="7"/>
@@ -7515,17 +9778,15 @@
         <f t="shared" si="8"/>
         <v>132.82</v>
       </c>
-      <c r="BK20" s="7" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BL20" s="7" t="e">
-        <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BM20" s="6" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="BK20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BL20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="BM20" s="6">
+        <f t="shared" si="14"/>
+        <v>56.5</v>
       </c>
     </row>
   </sheetData>
@@ -7534,31 +9795,55 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:T20">
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="lessThan">
-      <formula>30</formula>
+    <cfRule type="cellIs" dxfId="7" priority="20" operator="equal">
+      <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="21" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="22" operator="between">
+      <formula>60</formula>
       <formula>70</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="23" operator="between">
       <formula>30</formula>
       <formula>40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="between">
-      <formula>60</formula>
+    <cfRule type="cellIs" dxfId="3" priority="24" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="25" operator="greaterThan">
       <formula>70</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
-      <formula>"N/A"</formula>
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="lessThan">
+      <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U20">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ2:AQ20">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BM2:BM20">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -7570,19 +9855,457 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ2:AQ20">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="AT2:BL20">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
       </colorScale>
     </cfRule>
+    <cfRule type="expression" dxfId="0" priority="7">
+      <formula>"IF ISNUMBER"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM2:BM20">
+  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="13" max="20" man="1"/>
+  </rowBreaks>
+  <colBreaks count="3" manualBreakCount="3">
+    <brk id="7" max="19" man="1"/>
+    <brk id="14" max="19" man="1"/>
+    <brk id="19" max="1048575" man="1"/>
+  </colBreaks>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>22.02</v>
+      </c>
+      <c r="C3">
+        <v>20.14</v>
+      </c>
+      <c r="D3">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="E3">
+        <v>8.7899999999999991</v>
+      </c>
+      <c r="F3">
+        <f>(B3+C3)/2</f>
+        <v>21.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>20.76</v>
+      </c>
+      <c r="C4">
+        <v>19.09</v>
+      </c>
+      <c r="D4">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="E4">
+        <v>8.35</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F23" si="0">(B4+C4)/2</f>
+        <v>19.925000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>24.96</v>
+      </c>
+      <c r="C5">
+        <v>22.42</v>
+      </c>
+      <c r="D5">
+        <v>11.2</v>
+      </c>
+      <c r="E5">
+        <v>9.8699999999999992</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>23.69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>25.58</v>
+      </c>
+      <c r="C6">
+        <v>21.6</v>
+      </c>
+      <c r="D6">
+        <v>11.5</v>
+      </c>
+      <c r="E6">
+        <v>9.93</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>23.59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>25.4</v>
+      </c>
+      <c r="C7">
+        <v>26.06</v>
+      </c>
+      <c r="D7">
+        <v>11.41</v>
+      </c>
+      <c r="E7">
+        <v>11.96</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>25.729999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>22.82</v>
+      </c>
+      <c r="C8">
+        <v>23.39</v>
+      </c>
+      <c r="D8">
+        <v>10.07</v>
+      </c>
+      <c r="E8">
+        <v>10.62</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>23.105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>23.14</v>
+      </c>
+      <c r="C9">
+        <v>22.92</v>
+      </c>
+      <c r="D9">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="E9">
+        <v>9.41</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>23.03</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>24.13</v>
+      </c>
+      <c r="C10">
+        <v>17.88</v>
+      </c>
+      <c r="D10">
+        <v>10.65</v>
+      </c>
+      <c r="E10">
+        <v>8.76</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>21.004999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>25.39</v>
+      </c>
+      <c r="C11">
+        <v>23.22</v>
+      </c>
+      <c r="D11">
+        <v>10.84</v>
+      </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>24.305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>25.22</v>
+      </c>
+      <c r="C12">
+        <v>21.75</v>
+      </c>
+      <c r="D12">
+        <v>11.19</v>
+      </c>
+      <c r="E12">
+        <v>8.86</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>23.484999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>24.1</v>
+      </c>
+      <c r="C13">
+        <v>23.94</v>
+      </c>
+      <c r="D13">
+        <v>10.51</v>
+      </c>
+      <c r="E13">
+        <v>10.55</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>24.020000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>26.07</v>
+      </c>
+      <c r="C14">
+        <v>26.45</v>
+      </c>
+      <c r="D14">
+        <v>12.14</v>
+      </c>
+      <c r="E14">
+        <v>12.46</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>26.259999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>22.31</v>
+      </c>
+      <c r="C15">
+        <v>21.33</v>
+      </c>
+      <c r="D15">
+        <v>9.43</v>
+      </c>
+      <c r="E15">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>21.82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>24.35</v>
+      </c>
+      <c r="C16">
+        <v>24.01</v>
+      </c>
+      <c r="D16">
+        <v>10.83</v>
+      </c>
+      <c r="E16">
+        <v>10.68</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>24.18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>26.63</v>
+      </c>
+      <c r="C17">
+        <v>24.13</v>
+      </c>
+      <c r="D17">
+        <v>11.3</v>
+      </c>
+      <c r="E17">
+        <v>10.49</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>25.38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="C18">
+        <v>19.059999999999999</v>
+      </c>
+      <c r="D18">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="E18">
+        <v>8.26</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>19.454999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>22.88</v>
+      </c>
+      <c r="C19">
+        <v>22.04</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>22.46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>29.3</v>
+      </c>
+      <c r="C20">
+        <v>27.26</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>28.28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>22.42</v>
+      </c>
+      <c r="C21">
+        <v>27.22</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>24.82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <f>AVERAGE(B3:B21)</f>
+        <v>24.070000000000004</v>
+      </c>
+      <c r="C23">
+        <f>AVERAGE(C3:C21)</f>
+        <v>22.837368421052631</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>23.453684210526319</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F3:F21">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -7594,16 +10317,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="14" max="20" man="1"/>
-  </rowBreaks>
-  <colBreaks count="3" manualBreakCount="3">
-    <brk id="7" max="19" man="1"/>
-    <brk id="14" max="19" man="1"/>
-    <brk id="19" max="1048575" man="1"/>
-  </colBreaks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>